<commit_message>
Update Bill Of Materialsi
</commit_message>
<xml_diff>
--- a/7347_Robot_BOM.xlsx
+++ b/7347_Robot_BOM.xlsx
@@ -41,15 +41,9 @@
     <t>QTY 1       surgical tubing</t>
   </si>
   <si>
-    <t>QTY 6       LEGO pieces</t>
-  </si>
-  <si>
     <t>Game Manual Pt 1:  &lt;R01&gt;</t>
   </si>
   <si>
-    <t>QTY 2       linear slides</t>
-  </si>
-  <si>
     <t>QTY 1       gaffer's tape</t>
   </si>
   <si>
@@ -77,9 +71,6 @@
     <t>QTY 1       Gorilla Tape</t>
   </si>
   <si>
-    <t>QTY 16     zip ties</t>
-  </si>
-  <si>
     <t>QTY 1       painter's tape</t>
   </si>
   <si>
@@ -87,6 +78,15 @@
   </si>
   <si>
     <t>Game Manual Pt 1:  &lt;R08.b&gt;</t>
+  </si>
+  <si>
+    <t>QTY 20     zip ties</t>
+  </si>
+  <si>
+    <t>QTY 25     LEGO pieces</t>
+  </si>
+  <si>
+    <t>QTY 4       linear slides</t>
   </si>
 </sst>
 </file>
@@ -183,11 +183,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,7 +460,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -471,7 +471,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -482,10 +482,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="12"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -549,7 +549,7 @@
     </row>
     <row r="7" spans="1:6" ht="14.25" customHeight="1">
       <c r="A7" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>5</v>
@@ -561,10 +561,10 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>7</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>8</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -573,10 +573,10 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="8" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -585,7 +585,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>5</v>
@@ -597,7 +597,7 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>5</v>
@@ -609,10 +609,10 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -621,7 +621,7 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>5</v>
@@ -633,7 +633,7 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>5</v>
@@ -645,10 +645,10 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -657,7 +657,7 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>5</v>
@@ -669,7 +669,7 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>5</v>
@@ -680,8 +680,8 @@
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="12" t="s">
-        <v>20</v>
+      <c r="A18" s="10" t="s">
+        <v>17</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Same exact update again :rage:
</commit_message>
<xml_diff>
--- a/7347_Robot_BOM.xlsx
+++ b/7347_Robot_BOM.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>FTC  Robot Bill of Materials</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>QTY 4       linear slides</t>
+  </si>
+  <si>
+    <t>QTY 1       duct tape</t>
   </si>
 </sst>
 </file>
@@ -460,7 +463,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -471,7 +474,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -691,7 +694,13 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" ht="12.75">
+    <row r="19" spans="1:6">
+      <c r="A19" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>5</v>
+      </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>

</xml_diff>